<commit_message>
Cambio en casos de prueba
</commit_message>
<xml_diff>
--- a/Pruebas/Testing.xlsx
+++ b/Pruebas/Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\Proyecto\Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E1D468-7FBC-4578-AE3C-684A84294131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47E88ED-4161-49A6-8494-9289C513C046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA18E821-FBED-465F-9074-D5456AD5FF38}"/>
+    <workbookView xWindow="10845" yWindow="4605" windowWidth="11820" windowHeight="11385" xr2:uid="{AA18E821-FBED-465F-9074-D5456AD5FF38}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>No</t>
   </si>
@@ -54,17 +54,128 @@
     <t>Pasos</t>
   </si>
   <si>
-    <t>Salida esperada</t>
-  </si>
-  <si>
     <t>Resultado esperado</t>
+  </si>
+  <si>
+    <t>CP_Login1</t>
+  </si>
+  <si>
+    <t>CP_Login2</t>
+  </si>
+  <si>
+    <t>CP_Login3</t>
+  </si>
+  <si>
+    <t>CP_Login4</t>
+  </si>
+  <si>
+    <t>CP_Login5</t>
+  </si>
+  <si>
+    <t>CP_Login6</t>
+  </si>
+  <si>
+    <t>CP_Login7</t>
+  </si>
+  <si>
+    <t>Iniciar sesion con los campos vacios</t>
+  </si>
+  <si>
+    <t>Iniciar sesion con el campo correo erroneo</t>
+  </si>
+  <si>
+    <t>Iniciar sesion con el campo contraseña erroneo</t>
+  </si>
+  <si>
+    <t>Iniciar sesion con campo de correo vacio y contraseña diligenciado</t>
+  </si>
+  <si>
+    <t>Iniciar sesion con campo de correo diligenciado y contraseña vacio</t>
+  </si>
+  <si>
+    <t>Iniciar sesion con datos erroneos</t>
+  </si>
+  <si>
+    <t>Iniciar sesion con datos verdaderos</t>
+  </si>
+  <si>
+    <t>CP_Register1</t>
+  </si>
+  <si>
+    <t>CP_Register2</t>
+  </si>
+  <si>
+    <t>CP_Register3</t>
+  </si>
+  <si>
+    <t>CP_Register4</t>
+  </si>
+  <si>
+    <t>CP_Register5</t>
+  </si>
+  <si>
+    <t>CP_Register6</t>
+  </si>
+  <si>
+    <t>CP_Register7</t>
+  </si>
+  <si>
+    <t>CP_Register8</t>
+  </si>
+  <si>
+    <t>CP_Register9</t>
+  </si>
+  <si>
+    <t>Registrar usuario con todos los campos vacios</t>
+  </si>
+  <si>
+    <t>Debe estar registrado el usuario</t>
+  </si>
+  <si>
+    <t>Debe contener los campos obligatorios</t>
+  </si>
+  <si>
+    <t>Yeison@MundoAnimal.com / 1000088550</t>
+  </si>
+  <si>
+    <t>Yeison@Mundo.com / 100008855</t>
+  </si>
+  <si>
+    <t>Null / Null</t>
+  </si>
+  <si>
+    <t>Null / 1000088550</t>
+  </si>
+  <si>
+    <t>Yeison@MundoAnimal.com / Null</t>
+  </si>
+  <si>
+    <t>Yeison@Animal.com / 10000088550</t>
+  </si>
+  <si>
+    <t>Yeison@MundoAnimal.com / 10008855</t>
+  </si>
+  <si>
+    <t>El usuario debe llenar los campos solicitados</t>
+  </si>
+  <si>
+    <t>74635215 / Juan / Martinez / 315698754 / CL 87 CR 31 67 / JuanM@gmail.com / 74635215</t>
+  </si>
+  <si>
+    <t>Salida</t>
+  </si>
+  <si>
+    <t>Ingreso al sistema</t>
+  </si>
+  <si>
+    <t>Corf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +187,20 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,11 +229,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -116,8 +242,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Texto explicativo" xfId="1" builtinId="53"/>
   </cellStyles>
@@ -433,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2CAF49-1716-467C-A32D-3B24F79E1959}">
   <dimension ref="B2:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,143 +600,277 @@
         <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>9</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>10</v>
       </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>11</v>
       </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>12</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>13</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>26</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{10A80549-5D26-4C64-A385-68962B45AD29}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{0DC63AB3-F8F7-49D4-B002-E0B395F78909}"/>
+    <hyperlink ref="F7" r:id="rId3" xr:uid="{56F688B5-3EA9-4719-A3E7-F2955C56D1EE}"/>
+    <hyperlink ref="F8" r:id="rId4" xr:uid="{24C57650-8B6C-49AA-8E9D-BEC7360B6553}"/>
+    <hyperlink ref="F9" r:id="rId5" xr:uid="{805826B3-B946-4604-B0D2-240CA244626D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>